<commit_message>
Presentacion del Modulo juegos de Mesa
</commit_message>
<xml_diff>
--- a/EJERCICIO 01 - 25-08-2023_Spadoni_Rodriguez_Mejia.xlsx
+++ b/EJERCICIO 01 - 25-08-2023_Spadoni_Rodriguez_Mejia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agus\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20329059651\Desktop\Trabajos_practicos_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2985ACD9-BC45-4AE4-9FAC-662940AA3837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715A1679-6BB7-44B3-A809-406B4F57A7A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HOJA DE DATOS" sheetId="1" r:id="rId1"/>
@@ -21,17 +21,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -873,24 +862,6 @@
     <xf numFmtId="168" fontId="0" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -906,17 +877,14 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="165" fontId="14" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="14" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -924,11 +892,32 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1486,6 +1475,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-86FD-4E4C-A4F9-577606C927F4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1512,6 +1506,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-86FD-4E4C-A4F9-577606C927F4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1538,6 +1537,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-86FD-4E4C-A4F9-577606C927F4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -4960,10 +4964,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:XFC24"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5021,7 +5026,7 @@
       </c>
       <c r="L2" s="22">
         <f ca="1">TODAY()</f>
-        <v>45193</v>
+        <v>45229</v>
       </c>
       <c r="N2" s="19" t="s">
         <v>50</v>
@@ -5051,7 +5056,7 @@
       </c>
       <c r="H3" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>25.326027397260273</v>
+        <v>25.424657534246574</v>
       </c>
       <c r="I3" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5090,7 +5095,7 @@
       </c>
       <c r="H4" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>68.835616438356169</v>
+        <v>68.93424657534247</v>
       </c>
       <c r="I4" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5132,7 +5137,7 @@
       </c>
       <c r="H5" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>59.838356164383562</v>
+        <v>59.936986301369863</v>
       </c>
       <c r="I5" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5174,7 +5179,7 @@
       </c>
       <c r="H6" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>32.978082191780821</v>
+        <v>33.076712328767123</v>
       </c>
       <c r="I6" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5216,7 +5221,7 @@
       </c>
       <c r="H7" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>38.276712328767125</v>
+        <v>38.375342465753427</v>
       </c>
       <c r="I7" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5258,7 +5263,7 @@
       </c>
       <c r="H8" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>50.673972602739724</v>
+        <v>50.772602739726025</v>
       </c>
       <c r="I8" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5294,7 +5299,7 @@
       </c>
       <c r="H9" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>28.057534246575344</v>
+        <v>28.156164383561645</v>
       </c>
       <c r="I9" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5330,7 +5335,7 @@
       </c>
       <c r="H10" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>27.545205479452054</v>
+        <v>27.643835616438356</v>
       </c>
       <c r="I10" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5366,7 +5371,7 @@
       </c>
       <c r="H11" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>40.964383561643835</v>
+        <v>41.063013698630137</v>
       </c>
       <c r="I11" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5402,7 +5407,7 @@
       </c>
       <c r="H12" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>37.221917808219175</v>
+        <v>37.320547945205476</v>
       </c>
       <c r="I12" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5438,7 +5443,7 @@
       </c>
       <c r="H13" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>30.046575342465754</v>
+        <v>30.145205479452056</v>
       </c>
       <c r="I13" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5474,7 +5479,7 @@
       </c>
       <c r="H14" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>53.679452054794524</v>
+        <v>53.778082191780825</v>
       </c>
       <c r="I14" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5510,7 +5515,7 @@
       </c>
       <c r="H15" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>34.361643835616441</v>
+        <v>34.460273972602742</v>
       </c>
       <c r="I15" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5546,7 +5551,7 @@
       </c>
       <c r="H16" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>33.128767123287673</v>
+        <v>33.227397260273975</v>
       </c>
       <c r="I16" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5582,7 +5587,7 @@
       </c>
       <c r="H17" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>23.657534246575342</v>
+        <v>23.756164383561643</v>
       </c>
       <c r="I17" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5618,7 +5623,7 @@
       </c>
       <c r="H18" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>27.8</v>
+        <v>27.898630136986302</v>
       </c>
       <c r="I18" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5654,7 +5659,7 @@
       </c>
       <c r="H19" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>43.87945205479452</v>
+        <v>43.978082191780821</v>
       </c>
       <c r="I19" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5690,7 +5695,7 @@
       </c>
       <c r="H20" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>41.252054794520546</v>
+        <v>41.350684931506848</v>
       </c>
       <c r="I20" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5726,7 +5731,7 @@
       </c>
       <c r="H21" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>24.745205479452054</v>
+        <v>24.843835616438355</v>
       </c>
       <c r="I21" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5762,7 +5767,7 @@
       </c>
       <c r="H22" s="25">
         <f ca="1">($L$2-Tabla_empleados[[#This Row],[FECHA DE NAC.]] )/365</f>
-        <v>49.506849315068493</v>
+        <v>49.605479452054794</v>
       </c>
       <c r="I22" s="37">
         <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
@@ -5788,9 +5793,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Hoja2"/>
   <dimension ref="A4:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
@@ -5806,14 +5812,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="D4" s="38" t="s">
+      <c r="B4" s="49"/>
+      <c r="D4" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="39"/>
+      <c r="E4" s="49"/>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
@@ -5846,14 +5852,14 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="39"/>
-      <c r="D9" s="38" t="s">
+      <c r="B9" s="49"/>
+      <c r="D9" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="39"/>
+      <c r="E9" s="49"/>
     </row>
     <row r="10" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
@@ -5927,21 +5933,21 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="39"/>
-      <c r="D17" s="38" t="s">
+      <c r="B17" s="49"/>
+      <c r="D17" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="39"/>
+      <c r="E17" s="49"/>
     </row>
     <row r="18" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="55">
+      <c r="A18" s="53">
         <f>COUNTIF(Tabla_empleados[AÑOS DE TRABAJO],"&gt;5")</f>
         <v>10</v>
       </c>
-      <c r="B18" s="56"/>
+      <c r="B18" s="54"/>
       <c r="D18" s="11" t="s">
         <v>40</v>
       </c>
@@ -5977,14 +5983,14 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="39"/>
-      <c r="D24" s="42" t="s">
+      <c r="B24" s="49"/>
+      <c r="D24" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="43"/>
+      <c r="E24" s="56"/>
     </row>
     <row r="25" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
@@ -5996,7 +6002,7 @@
       <c r="D25" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="44" t="s">
+      <c r="E25" s="38" t="s">
         <v>69</v>
       </c>
     </row>
@@ -6015,7 +6021,7 @@
         <f>SUMIF(Tabla_empleados[PROVINCIA],D26,Tabla_empleados[Sueldo en Pesos])</f>
         <v>10300000</v>
       </c>
-      <c r="F26" s="52" t="s">
+      <c r="F26" s="43" t="s">
         <v>31</v>
       </c>
     </row>
@@ -6034,7 +6040,7 @@
         <f>SUMIF(Tabla_empleados[PROVINCIA],D27,Tabla_empleados[Sueldo en Pesos])</f>
         <v>4800000</v>
       </c>
-      <c r="F27" s="52" t="s">
+      <c r="F27" s="43" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6053,7 +6059,7 @@
         <f>SUMIF(Tabla_empleados[PROVINCIA],D28,Tabla_empleados[Sueldo en Pesos])</f>
         <v>8650000</v>
       </c>
-      <c r="F28" s="52" t="s">
+      <c r="F28" s="43" t="s">
         <v>33</v>
       </c>
     </row>
@@ -6083,11 +6089,11 @@
         <f>'HOJA DE DATOS'!I8 / $B$46</f>
         <v>1512.7067365873336</v>
       </c>
-      <c r="D31" s="40" t="s">
+      <c r="D31" s="50" t="s">
         <v>52</v>
       </c>
       <c r="E31" s="51"/>
-      <c r="F31" s="41"/>
+      <c r="F31" s="52"/>
     </row>
     <row r="32" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="26" t="s">
@@ -6100,11 +6106,11 @@
       <c r="D32" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E32" s="49">
+      <c r="E32" s="44">
         <f>MAX(E26:E28)</f>
         <v>10300000</v>
       </c>
-      <c r="F32" s="50"/>
+      <c r="F32" s="45"/>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="26" t="s">
@@ -6117,11 +6123,11 @@
       <c r="D33" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="53" t="str">
+      <c r="E33" s="46" t="str">
         <f>VLOOKUP(E32,E26:F28,2,FALSE)</f>
         <v>Cordoba</v>
       </c>
-      <c r="F33" s="54"/>
+      <c r="F33" s="47"/>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="26" t="s">
@@ -6149,7 +6155,7 @@
         <f>'HOJA DE DATOS'!I13 / $B$46</f>
         <v>819.38281565147236</v>
       </c>
-      <c r="D36" s="46" t="s">
+      <c r="D36" s="40" t="s">
         <v>42</v>
       </c>
     </row>
@@ -6182,18 +6188,18 @@
         <f>'HOJA DE DATOS'!I15 / $B$46</f>
         <v>1512.7067365873336</v>
       </c>
-      <c r="D38" s="47">
+      <c r="D38" s="41">
         <v>11</v>
       </c>
-      <c r="E38" s="47" t="str">
+      <c r="E38" s="41" t="str">
         <f>VLOOKUP(D38,Tabla_empleados[],2,FALSE)</f>
         <v>Agustín</v>
       </c>
-      <c r="F38" s="47" t="str">
+      <c r="F38" s="41" t="str">
         <f>VLOOKUP(D38,Tabla_empleados[],6,FALSE)</f>
         <v>Administrativo</v>
       </c>
-      <c r="G38" s="48">
+      <c r="G38" s="42">
         <f>VLOOKUP(D38,Tabla_empleados[],9,FALSE)</f>
         <v>650000</v>
       </c>
@@ -6265,7 +6271,7 @@
       <c r="A46" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="B46" s="45" t="s">
+      <c r="B46" s="39" t="s">
         <v>71</v>
       </c>
     </row>
@@ -6305,19 +6311,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Hoja3"/>
   <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="39"/>
+      <c r="B2" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>